<commit_message>
Tried my best with a 2100 problem
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
   <si>
     <t>Day</t>
   </si>
@@ -485,6 +485,18 @@
   </si>
   <si>
     <t>Easy problem, good time I would say</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1920/problem/E</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>I tried my best but coudn't find the idea
+I then red the editorial a little, I got the principle
+so I want to solve it alone in a few days, I really need to start stepping 
+up and get good at 2000-2300 rating problems</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -501,10 +513,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -539,7 +551,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,18 +565,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -583,6 +595,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -593,14 +612,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,6 +626,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -622,22 +642,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,9 +671,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -675,7 +687,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,37 +699,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +747,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,19 +765,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -771,13 +813,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,73 +861,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -888,7 +900,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -897,22 +918,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -932,11 +938,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -971,118 +983,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1097,7 +1109,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1106,7 +1118,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1466,7 +1478,7 @@
   <dimension ref="A1:M99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -3263,18 +3275,32 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" ht="105" spans="1:11">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
+      <c r="E70" s="2">
+        <v>2100</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G70" s="2">
+        <v>100</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0</v>
+      </c>
+      <c r="I70" s="2">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="2"/>
@@ -3504,11 +3530,11 @@
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G88" s="2">
         <f>SUM(G1:G87)/60</f>
-        <v>34.9666666666667</v>
+        <v>36.6333333333333</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -3522,11 +3548,11 @@
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G89" s="2">
         <f>G88/MAX(A6:A87)</f>
-        <v>2.18541666666667</v>
+        <v>2.28958333333333</v>
       </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -3553,7 +3579,7 @@
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G91" s="2">
         <f>AVERAGEIFS(G:G,E:E,1700)</f>
@@ -3720,6 +3746,7 @@
     <hyperlink ref="F66" r:id="rId45" display="https://codeforces.com/contest/1611/problem/E1"/>
     <hyperlink ref="F68" r:id="rId46" display="https://codeforces.com/contest/1692/problem/H"/>
     <hyperlink ref="F69" r:id="rId47" display="https://codeforces.com/contest/915/problem/C"/>
+    <hyperlink ref="F70" r:id="rId48" display="https://codeforces.com/contest/1920/problem/E"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Solved 1700 problem with SegmentTree
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="152">
   <si>
     <t>Day</t>
   </si>
@@ -523,6 +523,17 @@
     <t>I upsolved problem D from last contest
 It was an ok problem, I had the main idea but
 unfortunately that I understood it wrong</t>
+  </si>
+  <si>
+    <t>If elements are gone one by one we can
+update easily the left and right closest
+neighbour</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1023/problem/D</t>
+  </si>
+  <si>
+    <t>Beautiful Segment Tree problem</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -576,9 +587,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -591,27 +609,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -623,16 +624,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -647,39 +664,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -691,16 +686,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -713,7 +724,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,7 +796,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,91 +868,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,61 +898,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -904,54 +915,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -985,12 +948,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1004,147 +1006,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1154,7 +1165,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1178,6 +1189,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1501,10 +1515,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M99"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="K87" sqref="K86:K87"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -3388,12 +3402,12 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" ht="60" spans="1:11">
+    <row r="74" ht="60" spans="1:12">
       <c r="A74" s="2">
         <v>18</v>
       </c>
       <c r="B74" s="2">
-        <v>1503</v>
+        <v>1606</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>143</v>
@@ -3408,7 +3422,7 @@
         <v>144</v>
       </c>
       <c r="G74" s="2">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="H74" s="2">
         <v>80</v>
@@ -3419,20 +3433,37 @@
       <c r="J74" s="2"/>
       <c r="K74" s="5" t="s">
         <v>145</v>
+      </c>
+      <c r="L74" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
+      <c r="D75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="2">
+        <v>1700</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G75" s="2">
+        <v>21</v>
+      </c>
+      <c r="H75" s="2">
+        <v>100</v>
+      </c>
+      <c r="I75" s="2">
+        <v>100</v>
+      </c>
       <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
+      <c r="K75" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="2"/>
@@ -3596,13 +3627,8 @@
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
-      <c r="F88" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G88" s="2">
-        <f>SUM(G1:G87)/60</f>
-        <v>38.4833333333333</v>
-      </c>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
@@ -3614,13 +3640,8 @@
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
-      <c r="F89" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G89" s="2">
-        <f>G88/MAX(A6:A87)</f>
-        <v>2.13796296296296</v>
-      </c>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
@@ -3645,13 +3666,8 @@
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
-      <c r="F91" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G91" s="2">
-        <f>AVERAGEIFS(G:G,E:E,1700)</f>
-        <v>30.7222222222222</v>
-      </c>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
@@ -3741,8 +3757,13 @@
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
+      <c r="F98" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G98" s="2">
+        <f>SUM(G1:G97)/60</f>
+        <v>39.1666666666667</v>
+      </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
@@ -3754,12 +3775,152 @@
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
+      <c r="F99" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G99" s="2">
+        <f>G98/MAX(A6:A97)</f>
+        <v>2.17592592592593</v>
+      </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G101" s="2">
+        <f>AVERAGEIFS(G:G,E:E,1700)</f>
+        <v>30.4594594594595</v>
+      </c>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+      <c r="K107" s="2"/>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3816,6 +3977,7 @@
     <hyperlink ref="F70" r:id="rId48" display="https://codeforces.com/contest/1920/problem/E"/>
     <hyperlink ref="F72" r:id="rId49" display="https://codeforces.com/contest/1922"/>
     <hyperlink ref="F74" r:id="rId50" display="https://codeforces.com/contest/1922/problem/D"/>
+    <hyperlink ref="F75" r:id="rId51" display="https://codeforces.com/contest/1023/problem/D"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Stuck on a problem
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="156">
   <si>
     <t>Day</t>
   </si>
@@ -540,6 +540,14 @@
   </si>
   <si>
     <t>Standard Bitmask problem, kinda slow time</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1896/problem/D</t>
+  </si>
+  <si>
+    <t>I got stuck in a wrong aproch, I red a little bit
+from editorial so I don't know the solution but
+I know that it's not done with segment tree</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -556,10 +564,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -593,6 +601,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -601,7 +631,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -616,41 +662,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -670,21 +685,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -704,22 +728,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -730,7 +738,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -742,13 +750,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,7 +786,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,19 +798,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,37 +870,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,19 +900,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,49 +912,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,6 +929,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -965,15 +997,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1006,162 +1029,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1520,8 +1528,8 @@
   <sheetPr/>
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C70" workbookViewId="0">
+      <selection activeCell="I86" sqref="I82:I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -3497,18 +3505,28 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" ht="75" spans="1:11">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
+      <c r="D77" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="2">
+        <v>1700</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G77" s="2">
+        <v>56</v>
+      </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
+      <c r="K77" s="5" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="2"/>
@@ -3777,11 +3795,11 @@
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G98" s="2">
         <f>SUM(G1:G97)/60</f>
-        <v>39.7</v>
+        <v>40.6333333333333</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -3795,11 +3813,11 @@
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G99" s="2">
         <f>G98/MAX(A6:A97)</f>
-        <v>2.20555555555556</v>
+        <v>2.25740740740741</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
@@ -3826,11 +3844,11 @@
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G101" s="2">
         <f>AVERAGEIFS(G:G,E:E,1700)</f>
-        <v>30.5</v>
+        <v>31.1538461538462</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
@@ -3998,6 +4016,7 @@
     <hyperlink ref="F74" r:id="rId50" display="https://codeforces.com/contest/1922/problem/D"/>
     <hyperlink ref="F75" r:id="rId51" display="https://codeforces.com/contest/1023/problem/D"/>
     <hyperlink ref="F76" r:id="rId52" display="https://codeforces.com/problemset/problem/1903/D1"/>
+    <hyperlink ref="F77" r:id="rId53" display="https://codeforces.com/contest/1896/problem/D"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Finished Partial Sums problem
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="182">
   <si>
     <t>Day</t>
   </si>
@@ -640,6 +640,14 @@
     <t>If in a matrix a cell  has Manhatan 
 Distance x then it's on the x-th secondary 
 diagonal</t>
+  </si>
+  <si>
+    <t>https://www.pbinfo.ro/probleme/4475/livada3</t>
+  </si>
+  <si>
+    <t>It was done using partial sums, nice problem
+I kinda new the way of solving but it was a little
+more implementation than usual</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -658,8 +666,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -693,9 +701,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -716,11 +723,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -732,9 +769,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -749,21 +785,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -777,16 +799,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -800,7 +815,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -813,13 +828,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -830,7 +838,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -842,61 +862,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -908,31 +892,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -950,31 +910,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -986,7 +952,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1004,13 +1000,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,6 +1029,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1039,11 +1056,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1058,16 +1081,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1098,21 +1121,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1126,142 +1134,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1271,7 +1279,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1298,9 +1306,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1621,10 +1626,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M109"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="I87" sqref="I87"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -3892,22 +3897,36 @@
       <c r="K87" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L87" s="9" t="s">
+      <c r="L87" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" ht="75" spans="1:11">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="D88" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
+      <c r="F88" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G88" s="2">
+        <v>55</v>
+      </c>
+      <c r="H88" s="2">
+        <v>100</v>
+      </c>
+      <c r="I88" s="2">
+        <v>100</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="2"/>
@@ -4032,13 +4051,8 @@
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
-      <c r="F98" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="G98" s="2">
-        <f>SUM(G1:G97)/60</f>
-        <v>48.6833333333333</v>
-      </c>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
@@ -4050,13 +4064,8 @@
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
-      <c r="F99" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G99" s="2">
-        <f>G98/MAX(A6:A97)</f>
-        <v>2.43416666666667</v>
-      </c>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
@@ -4081,13 +4090,8 @@
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
-      <c r="F101" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G101" s="2">
-        <f>AVERAGEIFS(G:G,E:E,1700)</f>
-        <v>32</v>
-      </c>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
@@ -4177,8 +4181,13 @@
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G108" s="2">
+        <f>SUM(G1:G107)/60</f>
+        <v>49.6</v>
+      </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
@@ -4190,12 +4199,152 @@
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
+      <c r="F109" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G109" s="2">
+        <f>G108/MAX(A6:A107)</f>
+        <v>2.48</v>
+      </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G111" s="2">
+        <f>AVERAGEIFS(G:G,E:E,1700)</f>
+        <v>32</v>
+      </c>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+    </row>
+    <row r="112" spans="1:11">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+    </row>
+    <row r="113" spans="1:11">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+    </row>
+    <row r="114" spans="1:11">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+    </row>
+    <row r="115" spans="1:11">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+    </row>
+    <row r="116" spans="1:11">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+    </row>
+    <row r="117" spans="1:11">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+    </row>
+    <row r="118" spans="1:11">
+      <c r="A118" s="2"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+    </row>
+    <row r="119" spans="1:11">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4263,6 +4412,7 @@
     <hyperlink ref="F85" r:id="rId59" display="https://codeforces.com/contest/294/problem/B"/>
     <hyperlink ref="F86" r:id="rId60" display="https://codeforces.com/contest/1131/problem/F"/>
     <hyperlink ref="F87" r:id="rId61" display="https://www.pbinfo.ro/probleme/4564/douadrumuri"/>
+    <hyperlink ref="F88" r:id="rId62" display="https://www.pbinfo.ro/probleme/4475/livada3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Participated in Div2 contest and now I have rating 1737
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="208">
   <si>
     <t>Day</t>
   </si>
@@ -724,6 +724,16 @@
   <si>
     <t>Just a heavy implementation problem
 with some nice logic, kinda slow time but yeah...</t>
+  </si>
+  <si>
+    <t>27/01/2024</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1925</t>
+  </si>
+  <si>
+    <t>Got place 457/18600, with +126 rating change
+and performance of a 1910 rated coder</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -740,10 +750,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -777,25 +787,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -803,43 +796,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,6 +817,52 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -868,23 +870,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -904,6 +907,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -914,13 +924,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,61 +948,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1004,31 +972,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,7 +1020,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,43 +1080,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,26 +1118,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1149,20 +1144,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1178,6 +1179,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1210,142 +1220,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1704,8 +1714,8 @@
   <sheetPr/>
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="H107" sqref="H107"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C90" workbookViewId="0">
+      <selection activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -4312,18 +4322,36 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11">
-      <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
+    <row r="101" ht="45" spans="1:11">
+      <c r="A101" s="2">
+        <v>23</v>
+      </c>
+      <c r="B101" s="2">
+        <v>1737</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
+      <c r="F101" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G101" s="2">
+        <v>120</v>
+      </c>
+      <c r="H101" s="2">
+        <v>100</v>
+      </c>
+      <c r="I101" s="2">
+        <v>100</v>
+      </c>
       <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
+      <c r="K101" s="5" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="2"/>
@@ -4540,11 +4568,11 @@
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="G118" s="2">
         <f>SUM(G1:G117)/60</f>
-        <v>54.4333333333333</v>
+        <v>56.4333333333333</v>
       </c>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
@@ -4558,11 +4586,11 @@
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G119" s="2">
         <f>G118/MAX(A6:A117)</f>
-        <v>2.47424242424242</v>
+        <v>2.4536231884058</v>
       </c>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
@@ -4589,7 +4617,7 @@
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G121" s="2">
         <f>AVERAGEIFS(G:G,E:E,1700)</f>
@@ -4780,6 +4808,7 @@
     <hyperlink ref="F97" r:id="rId69" display="https://codeforces.com/problemset/problem/382/C"/>
     <hyperlink ref="F98" r:id="rId70" display="https://codeforces.com/problemset/problem/980/C"/>
     <hyperlink ref="F99" r:id="rId71" display="https://codeforces.com/problemset/problem/734/D"/>
+    <hyperlink ref="F101" r:id="rId72" display="https://codeforces.com/contest/1925"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Solved 2 virtual contests
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="213">
   <si>
     <t>Day</t>
   </si>
@@ -734,6 +734,24 @@
   <si>
     <t>Got place 457/18600, with +126 rating change
 and performance of a 1910 rated coder</t>
+  </si>
+  <si>
+    <t>29/01/2024</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1551</t>
+  </si>
+  <si>
+    <t>Participated virtually in div3 contest with a good
+performance</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1553</t>
+  </si>
+  <si>
+    <t>I participated in this virtual contest
+and took place 1414 with a performance of a 
+1820</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -750,10 +768,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -787,61 +805,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -854,9 +827,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -870,11 +843,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -887,7 +897,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,6 +924,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -924,7 +942,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,175 +1116,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1115,6 +1133,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1142,17 +1180,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1164,30 +1191,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1215,147 +1218,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1714,8 +1732,8 @@
   <sheetPr/>
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C90" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C94" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -4366,31 +4384,61 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11">
-      <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
+    <row r="103" ht="45" spans="1:11">
+      <c r="A103" s="2">
+        <v>24</v>
+      </c>
+      <c r="B103" s="2">
+        <v>1737</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
+      <c r="F103" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G103" s="2">
+        <v>120</v>
+      </c>
+      <c r="H103" s="2">
+        <v>100</v>
+      </c>
+      <c r="I103" s="2">
+        <v>100</v>
+      </c>
       <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="K103" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="104" ht="60" spans="1:11">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
+      <c r="D104" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
+      <c r="F104" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G104" s="2">
+        <v>120</v>
+      </c>
+      <c r="H104" s="2">
+        <v>100</v>
+      </c>
+      <c r="I104" s="2">
+        <v>100</v>
+      </c>
       <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
+      <c r="K104" s="5" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="2"/>
@@ -4568,11 +4616,11 @@
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="G118" s="2">
         <f>SUM(G1:G117)/60</f>
-        <v>56.4333333333333</v>
+        <v>60.4333333333333</v>
       </c>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
@@ -4586,11 +4634,11 @@
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G119" s="2">
         <f>G118/MAX(A6:A117)</f>
-        <v>2.4536231884058</v>
+        <v>2.51805555555556</v>
       </c>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
@@ -4617,7 +4665,7 @@
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="G121" s="2">
         <f>AVERAGEIFS(G:G,E:E,1700)</f>
@@ -4809,6 +4857,8 @@
     <hyperlink ref="F98" r:id="rId70" display="https://codeforces.com/problemset/problem/980/C"/>
     <hyperlink ref="F99" r:id="rId71" display="https://codeforces.com/problemset/problem/734/D"/>
     <hyperlink ref="F101" r:id="rId72" display="https://codeforces.com/contest/1925"/>
+    <hyperlink ref="F104" r:id="rId73" display="https://codeforces.com/contest/1553"/>
+    <hyperlink ref="F103" r:id="rId74" display="https://codeforces.com/contest/1551"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Solved two 1800 problems and learned about 0-1 BFS
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="248">
   <si>
     <t>Day</t>
   </si>
@@ -853,6 +853,28 @@
 this. Also I liked the idea for F even though
 it's not 100% a correct solution but I guess it works 
 as there are no hacks. Will upsolve D and F</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1721/problem/D</t>
+  </si>
+  <si>
+    <t>Pretty standard problem</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1063/B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I solved this with an ugly BFS that almost timed
+out.. </t>
+  </si>
+  <si>
+    <t>I solved previous problem the right way
+and I learned for the first time about 0-1 BFS. 
+It was an amazing solution</t>
+  </si>
+  <si>
+    <t>I learned about 0-1 BFS where edges can
+have only 2 different weights.</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -872,10 +894,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -910,15 +932,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -932,22 +946,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -957,6 +964,21 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -972,23 +994,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1009,17 +1022,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1030,8 +1043,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1046,7 +1068,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,13 +1098,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1082,13 +1122,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1112,31 +1164,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1148,19 +1206,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1178,55 +1242,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1237,21 +1259,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1279,6 +1286,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1290,21 +1312,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1337,147 +1344,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1487,7 +1509,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1514,6 +1536,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1834,10 +1859,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M139"/>
+  <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="K119" sqref="K119"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -4946,43 +4971,92 @@
       <c r="K120" s="2"/>
     </row>
     <row r="121" spans="1:11">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
-      <c r="J121" s="2"/>
-      <c r="K121" s="2"/>
-    </row>
-    <row r="122" spans="1:11">
+      <c r="A121" s="2">
+        <v>29</v>
+      </c>
+      <c r="B121" s="2">
+        <v>1737</v>
+      </c>
+      <c r="C121" s="3">
+        <v>45445</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E121" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G121" s="2">
+        <v>25</v>
+      </c>
+      <c r="H121" s="2">
+        <v>100</v>
+      </c>
+      <c r="I121" s="2">
+        <v>100</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="122" ht="45" spans="1:11">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
-      <c r="J122" s="2"/>
-      <c r="K122" s="2"/>
-    </row>
-    <row r="123" spans="1:11">
+      <c r="D122" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E122" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G122" s="2">
+        <v>45</v>
+      </c>
+      <c r="H122" s="2">
+        <v>100</v>
+      </c>
+      <c r="I122" s="2">
+        <v>100</v>
+      </c>
+      <c r="J122" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="K122" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="123" ht="60" spans="1:12">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
+      <c r="D123" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
-      <c r="G123" s="2"/>
+      <c r="F123" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G123" s="2">
+        <v>17</v>
+      </c>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
       <c r="J123" s="2"/>
-      <c r="K123" s="2"/>
+      <c r="K123" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="L123" s="9" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="124" spans="1:11">
       <c r="A124" s="2"/>
@@ -5042,13 +5116,8 @@
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
-      <c r="F128" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="G128" s="2">
-        <f>SUM(G1:G127)/60</f>
-        <v>70.7</v>
-      </c>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
       <c r="J128" s="2"/>
@@ -5060,13 +5129,8 @@
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
-      <c r="F129" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="G129" s="2">
-        <f>G128/MAX(A6:A127)</f>
-        <v>2.525</v>
-      </c>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129" s="2"/>
@@ -5091,13 +5155,8 @@
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
-      <c r="F131" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="G131" s="2">
-        <f>AVERAGEIFS(G:G,E:E,1700)</f>
-        <v>31.58</v>
-      </c>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
       <c r="J131" s="2"/>
@@ -5109,13 +5168,8 @@
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
-      <c r="F132" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G132" s="2">
-        <f>AVERAGEIFS(G:G,E:E,1800)</f>
-        <v>45.1666666666667</v>
-      </c>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
       <c r="J132" s="2"/>
@@ -5211,6 +5265,234 @@
       <c r="I139" s="2"/>
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
+    </row>
+    <row r="140" spans="1:11">
+      <c r="A140" s="2"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+    </row>
+    <row r="141" spans="1:11">
+      <c r="A141" s="2"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+      <c r="J141" s="2"/>
+      <c r="K141" s="2"/>
+    </row>
+    <row r="142" spans="1:11">
+      <c r="A142" s="2"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2"/>
+      <c r="K142" s="2"/>
+    </row>
+    <row r="143" spans="1:11">
+      <c r="A143" s="2"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+      <c r="H143" s="2"/>
+      <c r="I143" s="2"/>
+      <c r="J143" s="2"/>
+      <c r="K143" s="2"/>
+    </row>
+    <row r="144" spans="1:11">
+      <c r="A144" s="2"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G144" s="2">
+        <f>SUM(G1:G143)/60</f>
+        <v>72.15</v>
+      </c>
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+      <c r="J144" s="2"/>
+      <c r="K144" s="2"/>
+    </row>
+    <row r="145" spans="1:11">
+      <c r="A145" s="2"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G145" s="2">
+        <f>G144/MAX(A6:A143)</f>
+        <v>2.48793103448276</v>
+      </c>
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+      <c r="J145" s="2"/>
+      <c r="K145" s="2"/>
+    </row>
+    <row r="146" spans="1:11">
+      <c r="A146" s="2"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2"/>
+      <c r="K146" s="2"/>
+    </row>
+    <row r="147" spans="1:11">
+      <c r="A147" s="2"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G147" s="2">
+        <f>AVERAGEIFS(G:G,E:E,1700)</f>
+        <v>31.58</v>
+      </c>
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+      <c r="J147" s="2"/>
+      <c r="K147" s="2"/>
+    </row>
+    <row r="148" spans="1:11">
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G148" s="2">
+        <f>AVERAGEIFS(G:G,E:E,1800)</f>
+        <v>42.625</v>
+      </c>
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+      <c r="J148" s="2"/>
+      <c r="K148" s="2"/>
+    </row>
+    <row r="149" spans="1:11">
+      <c r="A149" s="2"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+      <c r="H149" s="2"/>
+      <c r="I149" s="2"/>
+      <c r="J149" s="2"/>
+      <c r="K149" s="2"/>
+    </row>
+    <row r="150" spans="1:11">
+      <c r="A150" s="2"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+      <c r="H150" s="2"/>
+      <c r="I150" s="2"/>
+      <c r="J150" s="2"/>
+      <c r="K150" s="2"/>
+    </row>
+    <row r="151" spans="1:11">
+      <c r="A151" s="2"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+      <c r="H151" s="2"/>
+      <c r="I151" s="2"/>
+      <c r="J151" s="2"/>
+      <c r="K151" s="2"/>
+    </row>
+    <row r="152" spans="1:11">
+      <c r="A152" s="2"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+      <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+      <c r="J152" s="2"/>
+      <c r="K152" s="2"/>
+    </row>
+    <row r="153" spans="1:11">
+      <c r="A153" s="2"/>
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2"/>
+      <c r="H153" s="2"/>
+      <c r="I153" s="2"/>
+      <c r="J153" s="2"/>
+      <c r="K153" s="2"/>
+    </row>
+    <row r="154" spans="1:11">
+      <c r="A154" s="2"/>
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2"/>
+      <c r="K154" s="2"/>
+    </row>
+    <row r="155" spans="1:11">
+      <c r="A155" s="2"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+      <c r="J155" s="2"/>
+      <c r="K155" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5302,6 +5584,9 @@
     <hyperlink ref="F117" r:id="rId83" display="https://www.codechef.com/problems/FRIENDGR"/>
     <hyperlink ref="F118" r:id="rId84" display="https://www.codechef.com/problems/FIBOSEQ"/>
     <hyperlink ref="F119" r:id="rId85" display="https://atcoder.jp/contests/abc339"/>
+    <hyperlink ref="F121" r:id="rId86" display="https://codeforces.com/contest/1721/problem/D"/>
+    <hyperlink ref="F122" r:id="rId87" display="https://codeforces.com/problemset/problem/1063/B" tooltip="https://codeforces.com/problemset/problem/1063/B"/>
+    <hyperlink ref="F123" r:id="rId87" display="https://codeforces.com/problemset/problem/1063/B"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Worked on 2000 rated problem
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="256">
   <si>
     <t>Day</t>
   </si>
@@ -902,6 +902,15 @@
 rently it's a way easier one, I didn't fully 
 understanded it but I will try tonight when going
 to sleep</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1831/problem/D</t>
+  </si>
+  <si>
+    <t>I tried to solve this but got time 
+limit exceed on test 3.. I got 70% of the ideas but
+still need some optimizations, I added this to the 
+queue of unsolved problems</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -921,9 +930,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -966,23 +975,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -990,7 +984,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1004,14 +998,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1020,7 +1006,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1036,15 +1030,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1065,9 +1058,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1083,6 +1084,14 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1101,25 +1110,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1137,7 +1128,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1149,19 +1242,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1173,91 +1272,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1269,13 +1284,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1304,24 +1313,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1333,21 +1324,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1381,8 +1357,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1391,142 +1400,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1885,8 +1894,8 @@
   <sheetPr/>
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="K127" sqref="K127"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="K130" sqref="K130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -5175,18 +5184,36 @@
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="1:11">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2"/>
+    <row r="128" ht="90" spans="1:11">
+      <c r="A128" s="2">
+        <v>31</v>
+      </c>
+      <c r="B128" s="2">
+        <v>1737</v>
+      </c>
+      <c r="C128" s="3">
+        <v>45506</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E128" s="2">
+        <v>200</v>
+      </c>
+      <c r="F128" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G128" s="2">
+        <v>75</v>
+      </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
-      <c r="J128" s="2"/>
-      <c r="K128" s="2"/>
+      <c r="J128" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K128" s="5" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="129" spans="1:11">
       <c r="A129" s="2"/>
@@ -5390,11 +5417,11 @@
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
       <c r="F144" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G144" s="2">
         <f>SUM(G1:G143)/60</f>
-        <v>73.8333333333333</v>
+        <v>75.0833333333333</v>
       </c>
       <c r="H144" s="2"/>
       <c r="I144" s="2"/>
@@ -5408,11 +5435,11 @@
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
       <c r="F145" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G145" s="2">
         <f>G144/MAX(A6:A143)</f>
-        <v>2.46111111111111</v>
+        <v>2.42204301075269</v>
       </c>
       <c r="H145" s="2"/>
       <c r="I145" s="2"/>
@@ -5439,7 +5466,7 @@
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
       <c r="F147" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G147" s="2">
         <f>AVERAGEIFS(G:G,E:E,1700)</f>
@@ -5457,7 +5484,7 @@
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
       <c r="F148" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G148" s="2">
         <f>AVERAGEIFS(G:G,E:E,1800)</f>
@@ -5654,6 +5681,7 @@
     <hyperlink ref="F123" r:id="rId87" display="https://codeforces.com/problemset/problem/1063/B"/>
     <hyperlink ref="F125" r:id="rId88" display="https://codeforces.com/contest/1548/problem/B"/>
     <hyperlink ref="F126" r:id="rId89" display="https://codeforces.com/contest/1705/problem/D"/>
+    <hyperlink ref="F128" r:id="rId90" display="https://codeforces.com/contest/1831/problem/D"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Found out about cool Number Theory property
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="278">
   <si>
     <t>Day</t>
   </si>
@@ -978,6 +978,16 @@
   <si>
     <t>Good problem, I had a bad bug because of
 an untinked soution so it costed me some time</t>
+  </si>
+  <si>
+    <t>https://www.pbinfo.ro/probleme/3849/exponentiere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I found out that a^n % p ==
+ a ^ (n % (p - 1)) % p </t>
+  </si>
+  <si>
+    <t>a^n % p == a ^ (n % (p - 1)) % p</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -997,10 +1007,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1035,15 +1045,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1054,6 +1063,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1073,7 +1089,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1087,16 +1103,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1110,8 +1134,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1125,38 +1157,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1171,13 +1181,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1189,7 +1199,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1207,7 +1235,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1219,7 +1247,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1231,31 +1277,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1267,13 +1289,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1285,25 +1319,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1315,43 +1355,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1362,21 +1372,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1405,6 +1400,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1422,19 +1443,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1442,23 +1467,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1467,118 +1477,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1587,22 +1597,22 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1612,7 +1622,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1639,6 +1649,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1961,8 +1974,8 @@
   <sheetPr/>
   <dimension ref="A1:M165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C128" workbookViewId="0">
-      <selection activeCell="L140" sqref="L140"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="E128" workbookViewId="0">
+      <selection activeCell="L142" sqref="L142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -5570,18 +5583,35 @@
         <v>270</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" ht="30" spans="1:12">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
+      <c r="D141" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
-      <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
-      <c r="I141" s="2"/>
-      <c r="J141" s="2"/>
-      <c r="K141" s="2"/>
+      <c r="F141" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="G141" s="2">
+        <v>20</v>
+      </c>
+      <c r="H141" s="2">
+        <v>0</v>
+      </c>
+      <c r="I141" s="2">
+        <v>100</v>
+      </c>
+      <c r="J141" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K141" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="L141" s="9" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="142" spans="1:11">
       <c r="A142" s="2"/>
@@ -5746,11 +5776,11 @@
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
       <c r="F154" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G154" s="2">
         <f>SUM(G1:G153)/60</f>
-        <v>84.2666666666667</v>
+        <v>84.6</v>
       </c>
       <c r="H154" s="2"/>
       <c r="I154" s="2"/>
@@ -5764,11 +5794,11 @@
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
       <c r="F155" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="G155" s="2">
         <f>G154/MAX(A6:A153)</f>
-        <v>1.95968992248062</v>
+        <v>1.96744186046512</v>
       </c>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
@@ -5795,7 +5825,7 @@
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
       <c r="F157" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G157" s="2">
         <f>AVERAGEIFS(G:G,E:E,1700)</f>
@@ -5813,7 +5843,7 @@
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G158" s="2">
         <f>AVERAGEIFS(G:G,E:E,1800)</f>
@@ -6018,6 +6048,7 @@
     <hyperlink ref="F133" r:id="rId95" display="https://codeforces.com/problemset/problem/1179/B"/>
     <hyperlink ref="F139" r:id="rId96" display="https://www.pbinfo.ro/probleme/4407/partitura"/>
     <hyperlink ref="F140" r:id="rId97" display="https://www.pbinfo.ro/probleme/4394/fotbal2"/>
+    <hyperlink ref="F141" r:id="rId98" display="https://www.pbinfo.ro/probleme/3849/exponentiere"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Solved easy OJI problem
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="292">
   <si>
     <t>Day</t>
   </si>
@@ -1031,6 +1031,12 @@
     <t>Great problem for memory optimization, I just
 got a small hint on compressing the needed
 memory, nothing else</t>
+  </si>
+  <si>
+    <t>https://www.pbinfo.ro/probleme/4409/castel4</t>
+  </si>
+  <si>
+    <t>Easy Greedy Problem</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -1052,8 +1058,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1087,6 +1093,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1102,23 +1116,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1126,14 +1132,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1149,6 +1155,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1156,7 +1185,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1177,39 +1213,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1221,6 +1227,12 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1236,13 +1248,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1254,25 +1302,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1290,37 +1380,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1332,79 +1404,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1415,6 +1421,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1436,6 +1457,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -1443,27 +1473,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1492,26 +1511,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1520,142 +1526,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2015,7 +2021,7 @@
   <dimension ref="A1:M172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="F152" sqref="F152"/>
+      <selection activeCell="L151" sqref="L151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -5853,17 +5859,35 @@
       <c r="K150" s="2"/>
     </row>
     <row r="151" spans="1:11">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
+      <c r="A151" s="2">
+        <v>46</v>
+      </c>
+      <c r="B151" s="2">
+        <v>1771</v>
+      </c>
       <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
+      <c r="D151" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E151" s="2"/>
-      <c r="F151" s="2"/>
-      <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
-      <c r="I151" s="2"/>
-      <c r="J151" s="2"/>
-      <c r="K151" s="2"/>
+      <c r="F151" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="G151" s="2">
+        <v>10</v>
+      </c>
+      <c r="H151" s="2">
+        <v>100</v>
+      </c>
+      <c r="I151" s="2">
+        <v>100</v>
+      </c>
+      <c r="J151" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K151" s="2" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="152" spans="1:11">
       <c r="A152" s="2"/>
@@ -5989,11 +6013,11 @@
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
       <c r="F161" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="G161" s="2">
         <f>SUM(G1:G160)/60</f>
-        <v>88.45</v>
+        <v>88.6166666666667</v>
       </c>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
@@ -6007,11 +6031,11 @@
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G162" s="2">
         <f>G161/MAX(A6:A160)</f>
-        <v>1.96555555555556</v>
+        <v>1.92644927536232</v>
       </c>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
@@ -6038,7 +6062,7 @@
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="G164" s="2">
         <f>AVERAGEIFS(G:G,E:E,1700)</f>
@@ -6056,7 +6080,7 @@
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
       <c r="F165" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="G165" s="2">
         <f>AVERAGEIFS(G:G,E:E,1800)</f>
@@ -6267,6 +6291,7 @@
     <hyperlink ref="F147" r:id="rId101" display="https://www.pbinfo.ro/probleme/594/eroziune"/>
     <hyperlink ref="F148" r:id="rId102" display="https://www.pbinfo.ro/probleme/3499/secv011"/>
     <hyperlink ref="F149" r:id="rId103" display="https://www.pbinfo.ro/probleme/4406/fibosnek"/>
+    <hyperlink ref="F151" r:id="rId104" display="https://www.pbinfo.ro/probleme/4409/castel4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Solved 7th grade OJI in 1:18 hours
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="301">
   <si>
     <t>Day</t>
   </si>
@@ -1055,6 +1055,16 @@
   </si>
   <si>
     <t>Interesting fast update greedy problem</t>
+  </si>
+  <si>
+    <t>https://www.pbinfo.ro/probleme/4398/palindrom4
+https://www.pbinfo.ro/probleme/4400/primprim</t>
+  </si>
+  <si>
+    <t>Greedy, Eratostene</t>
+  </si>
+  <si>
+    <t>Cool problems, nice ideas, but still easier</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -1075,9 +1085,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1111,23 +1121,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1143,14 +1146,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1171,6 +1182,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -1185,9 +1204,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1201,8 +1219,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1215,24 +1234,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1248,25 +1258,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1278,19 +1270,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1308,6 +1306,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1320,7 +1330,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1332,13 +1384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1350,7 +1396,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1362,19 +1408,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,49 +1432,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1442,11 +1452,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1462,15 +1511,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1509,177 +1549,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2036,10 +2046,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M192"/>
+  <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C148" workbookViewId="0">
-      <selection activeCell="H165" sqref="H165"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="K163" sqref="K163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -6005,18 +6015,32 @@
         <v>293</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" ht="30" spans="1:11">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
-      <c r="D156" s="2"/>
+      <c r="D156" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E156" s="2"/>
-      <c r="F156" s="2"/>
-      <c r="G156" s="2"/>
-      <c r="H156" s="2"/>
-      <c r="I156" s="2"/>
-      <c r="J156" s="2"/>
-      <c r="K156" s="2"/>
+      <c r="F156" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="G156" s="2">
+        <v>78</v>
+      </c>
+      <c r="H156" s="2">
+        <v>100</v>
+      </c>
+      <c r="I156" s="2">
+        <v>100</v>
+      </c>
+      <c r="J156" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="K156" s="2" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="157" spans="1:11">
       <c r="A157" s="2"/>
@@ -6024,7 +6048,7 @@
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
-      <c r="F157" s="2"/>
+      <c r="F157" s="4"/>
       <c r="G157" s="2"/>
       <c r="H157" s="2"/>
       <c r="I157" s="2"/>
@@ -6336,13 +6360,8 @@
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
-      <c r="F181" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="G181" s="2">
-        <f>SUM(G1:G180)/60</f>
-        <v>89.4833333333333</v>
-      </c>
+      <c r="F181" s="2"/>
+      <c r="G181" s="2"/>
       <c r="H181" s="2"/>
       <c r="I181" s="2"/>
       <c r="J181" s="2"/>
@@ -6355,11 +6374,11 @@
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="G182" s="2">
-        <f>G181/MAX(A6:A180)</f>
-        <v>1.90390070921986</v>
+        <f>SUM(G1:G181)/60</f>
+        <v>90.7833333333333</v>
       </c>
       <c r="H182" s="2"/>
       <c r="I182" s="2"/>
@@ -6372,8 +6391,13 @@
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
-      <c r="F183" s="2"/>
-      <c r="G183" s="2"/>
+      <c r="F183" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G183" s="2">
+        <f>G182/MAX(A6:A181)</f>
+        <v>1.93156028368794</v>
+      </c>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
       <c r="J183" s="2"/>
@@ -6385,13 +6409,8 @@
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
-      <c r="F184" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="G184" s="2">
-        <f>AVERAGEIFS(G:G,E:E,1700)</f>
-        <v>31.58</v>
-      </c>
+      <c r="F184" s="2"/>
+      <c r="G184" s="2"/>
       <c r="H184" s="2"/>
       <c r="I184" s="2"/>
       <c r="J184" s="2"/>
@@ -6404,11 +6423,11 @@
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="G185" s="2">
-        <f>AVERAGEIFS(G:G,E:E,1800)</f>
-        <v>42.7142857142857</v>
+        <f>AVERAGEIFS(G:G,E:E,1700)</f>
+        <v>31.58</v>
       </c>
       <c r="H185" s="2"/>
       <c r="I185" s="2"/>
@@ -6421,8 +6440,13 @@
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
-      <c r="F186" s="2"/>
-      <c r="G186" s="2"/>
+      <c r="F186" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G186" s="2">
+        <f>AVERAGEIFS(G:G,E:E,1800)</f>
+        <v>42.7142857142857</v>
+      </c>
       <c r="H186" s="2"/>
       <c r="I186" s="2"/>
       <c r="J186" s="2"/>
@@ -6505,6 +6529,19 @@
       <c r="I192" s="2"/>
       <c r="J192" s="2"/>
       <c r="K192" s="2"/>
+    </row>
+    <row r="193" spans="1:11">
+      <c r="A193" s="2"/>
+      <c r="B193" s="2"/>
+      <c r="C193" s="2"/>
+      <c r="D193" s="2"/>
+      <c r="E193" s="2"/>
+      <c r="F193" s="2"/>
+      <c r="G193" s="2"/>
+      <c r="H193" s="2"/>
+      <c r="I193" s="2"/>
+      <c r="J193" s="2"/>
+      <c r="K193" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6619,6 +6656,7 @@
     <hyperlink ref="F152" r:id="rId105" display="https://www.pbinfo.ro/probleme/4408/aeriana"/>
     <hyperlink ref="F154" r:id="rId106" display="https://www.pbinfo.ro/probleme/4402/ciocolata1"/>
     <hyperlink ref="F155" r:id="rId107" display="https://www.pbinfo.ro/probleme/4405/unificare"/>
+    <hyperlink ref="F156" r:id="rId108" display="https://www.pbinfo.ro/probleme/4398/palindrom4&#10;https://www.pbinfo.ro/probleme/4400/primprim" tooltip="https://www.pbinfo.ro/probleme/4398/palindrom4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Solved 12th grade OJI problem
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="303">
   <si>
     <t>Day</t>
   </si>
@@ -1065,6 +1065,13 @@
   </si>
   <si>
     <t>Cool problems, nice ideas, but still easier</t>
+  </si>
+  <si>
+    <t>https://www.pbinfo.ro/probleme/4411/veri</t>
+  </si>
+  <si>
+    <t>Shortest path and road building, nice problem
+overall</t>
   </si>
   <si>
     <t>Total time spent this year in hours:</t>
@@ -1084,10 +1091,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1121,6 +1128,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1129,10 +1145,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1144,9 +1160,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1160,8 +1190,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1176,14 +1207,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1197,8 +1220,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1211,29 +1235,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1241,11 +1242,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1258,7 +1265,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1270,7 +1289,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1288,73 +1367,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1366,7 +1397,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1378,7 +1409,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1390,49 +1433,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1449,21 +1456,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1484,8 +1476,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1495,7 +1489,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1532,11 +1526,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1544,8 +1551,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1557,139 +1564,139 @@
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2048,8 +2055,8 @@
   <sheetPr/>
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="K163" sqref="K163"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="I162" sqref="I162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -6042,18 +6049,32 @@
         <v>296</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" ht="45" spans="1:11">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
-      <c r="D157" s="2"/>
+      <c r="D157" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E157" s="2"/>
-      <c r="F157" s="4"/>
-      <c r="G157" s="2"/>
-      <c r="H157" s="2"/>
-      <c r="I157" s="2"/>
-      <c r="J157" s="2"/>
-      <c r="K157" s="2"/>
+      <c r="F157" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="G157" s="2">
+        <v>78</v>
+      </c>
+      <c r="H157" s="2">
+        <v>100</v>
+      </c>
+      <c r="I157" s="2">
+        <v>100</v>
+      </c>
+      <c r="J157" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="K157" s="5" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="158" spans="1:11">
       <c r="A158" s="2"/>
@@ -6374,11 +6395,11 @@
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="G182" s="2">
         <f>SUM(G1:G181)/60</f>
-        <v>90.7833333333333</v>
+        <v>92.0833333333333</v>
       </c>
       <c r="H182" s="2"/>
       <c r="I182" s="2"/>
@@ -6392,11 +6413,11 @@
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
       <c r="F183" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G183" s="2">
         <f>G182/MAX(A6:A181)</f>
-        <v>1.93156028368794</v>
+        <v>1.95921985815603</v>
       </c>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
@@ -6423,7 +6444,7 @@
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="G185" s="2">
         <f>AVERAGEIFS(G:G,E:E,1700)</f>
@@ -6441,7 +6462,7 @@
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="G186" s="2">
         <f>AVERAGEIFS(G:G,E:E,1800)</f>
@@ -6657,6 +6678,7 @@
     <hyperlink ref="F154" r:id="rId106" display="https://www.pbinfo.ro/probleme/4402/ciocolata1"/>
     <hyperlink ref="F155" r:id="rId107" display="https://www.pbinfo.ro/probleme/4405/unificare"/>
     <hyperlink ref="F156" r:id="rId108" display="https://www.pbinfo.ro/probleme/4398/palindrom4&#10;https://www.pbinfo.ro/probleme/4400/primprim" tooltip="https://www.pbinfo.ro/probleme/4398/palindrom4"/>
+    <hyperlink ref="F157" r:id="rId109" display="https://www.pbinfo.ro/probleme/4411/veri"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>